<commit_message>
Fix model emx files
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/MIAME-ENV_data.xlsx
+++ b/molgenis-model-registry/src/test/resources/MIAME-ENV_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="16440" tabRatio="664" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="16440" tabRatio="664" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="General features" sheetId="4" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="entities" sheetId="10" r:id="rId7"/>
     <sheet name="attributes" sheetId="11" r:id="rId8"/>
     <sheet name="packages" sheetId="12" r:id="rId9"/>
+    <sheet name="tags" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="84">
   <si>
     <t>name</t>
   </si>
@@ -237,6 +238,48 @@
   </si>
   <si>
     <t>http://nebc.nox.ac.uk/miame/MIAME1.6-envDraft-2.pdf</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>objectIRI</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>relationLabel</t>
+  </si>
+  <si>
+    <t>codeSystem</t>
+  </si>
+  <si>
+    <t>relationIRI</t>
+  </si>
+  <si>
+    <t>miameenv_home</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>http://molgenis.org/biobankconnect/link</t>
+  </si>
+  <si>
+    <t>miameenv_pub1</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed/16901223</t>
+  </si>
+  <si>
+    <t>Publication</t>
+  </si>
+  <si>
+    <t>miameenv_home,miameenv_pub1</t>
   </si>
 </sst>
 </file>
@@ -1191,20 +1234,20 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="148.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="148.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -1236,7 +1279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1273,6 +1316,95 @@
     <hyperlink ref="E2" r:id="rId1" tooltip="http://nebc.nox.ac.uk/miame/miame_env.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1284,13 +1416,13 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1298,7 +1430,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
@@ -1311,6 +1443,11 @@
     <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1322,9 +1459,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1334,6 +1471,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1345,9 +1487,9 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1355,7 +1497,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1363,7 +1505,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1371,7 +1513,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1379,7 +1521,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1389,6 +1531,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1400,13 +1547,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="77.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1417,7 +1564,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1430,6 +1577,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1441,13 +1593,13 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1458,7 +1610,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1471,6 +1623,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1478,17 +1635,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1659,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1510,7 +1667,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1518,7 +1675,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1526,7 +1683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1534,7 +1691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1542,7 +1699,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1553,6 +1710,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1564,16 +1726,16 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1623,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
@@ -1653,7 +1815,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1675,7 +1837,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1686,7 +1848,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1697,7 +1859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1708,7 +1870,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1719,7 +1881,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1730,7 +1892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1741,7 +1903,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1752,7 +1914,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1763,7 +1925,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1774,7 +1936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1791,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1811,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1825,7 +1987,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1845,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1856,7 +2018,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1873,7 +2035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1884,7 +2046,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1895,7 +2057,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1915,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1926,7 +2088,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1940,6 +2102,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1947,18 +2114,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1972,22 +2139,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
+      <c r="D2" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>